<commit_message>
add farmland position + add requirement file
</commit_message>
<xml_diff>
--- a/requirement.xlsx
+++ b/requirement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arrist\CMU\204113 Principles of Computing\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arrist\CMU\204113 Principles of Computing\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D9BF2C7-64EE-469B-9016-2302DAAE7ABF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A003A106-D7C9-45C0-8B53-8DA7E787FE88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="2895" windowWidth="28335" windowHeight="10365" activeTab="1" xr2:uid="{618F41DF-FE19-4F25-B31F-1E130881DE8A}"/>
+    <workbookView xWindow="-105" yWindow="2115" windowWidth="28335" windowHeight="10365" activeTab="1" xr2:uid="{618F41DF-FE19-4F25-B31F-1E130881DE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="image" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>main menu</t>
   </si>
@@ -176,6 +176,69 @@
   </si>
   <si>
     <t>every click in game</t>
+  </si>
+  <si>
+    <t>game icon</t>
+  </si>
+  <si>
+    <t>game icon(ซ้ายบน)</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>watering</t>
+  </si>
+  <si>
+    <t>change page</t>
+  </si>
+  <si>
+    <t>unknow</t>
+  </si>
+  <si>
+    <t>coin</t>
+  </si>
+  <si>
+    <t>watering in farm</t>
+  </si>
+  <si>
+    <t>lose</t>
+  </si>
+  <si>
+    <t>minigame</t>
+  </si>
+  <si>
+    <t>win</t>
+  </si>
+  <si>
+    <t>draw</t>
+  </si>
+  <si>
+    <t>theif_notice</t>
+  </si>
+  <si>
+    <t>steal crops</t>
+  </si>
+  <si>
+    <t>planting</t>
+  </si>
+  <si>
+    <t>เสียงวางผัก</t>
+  </si>
+  <si>
+    <t>planting crops</t>
+  </si>
+  <si>
+    <t>minigame starting</t>
+  </si>
+  <si>
+    <t>เตรียมเป่ายิงฉุบ???</t>
+  </si>
+  <si>
+    <t>มีมากกว่า 1 เพลงได้</t>
   </si>
 </sst>
 </file>
@@ -227,7 +290,46 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -537,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DA2599-C27D-4255-8280-6CD3A5A7DF81}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -550,7 +652,7 @@
     <col min="3" max="3" width="82.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -560,48 +662,66 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -611,8 +731,11 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -622,8 +745,11 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -633,8 +759,11 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -644,8 +773,11 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -655,48 +787,66 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -706,8 +856,11 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -717,24 +870,33 @@
       <c r="C18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -744,8 +906,11 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -755,8 +920,11 @@
       <c r="C22" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -766,8 +934,11 @@
       <c r="C23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -777,19 +948,61 @@
       <c r="C24" t="s">
         <v>39</v>
       </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{3B56BB6F-9D67-4460-AB8B-2B8C27459EF7}">
+            <xm:f>NOT(ISERROR(SEARCH(0,D1)))</xm:f>
+            <xm:f>0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B43348-8BF1-4962-9048-F23A20CD6675}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -799,7 +1012,7 @@
     <col min="3" max="3" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -809,32 +1022,160 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>47</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="0">
+      <formula>LEFT(D1,LEN("0"))="0"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
click on farmland now tell the crops info
</commit_message>
<xml_diff>
--- a/requirement.xlsx
+++ b/requirement.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arrist\CMU\204113 Principles of Computing\PROJECT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arrist\CMU\204113 Principles of Computing\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A003A106-D7C9-45C0-8B53-8DA7E787FE88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE752655-67D8-4A78-B25D-8D3ED2AA986D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="2115" windowWidth="28335" windowHeight="10365" activeTab="1" xr2:uid="{618F41DF-FE19-4F25-B31F-1E130881DE8A}"/>
+    <workbookView xWindow="16020" yWindow="1755" windowWidth="28335" windowHeight="10365" activeTab="2" xr2:uid="{618F41DF-FE19-4F25-B31F-1E130881DE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="image" sheetId="1" r:id="rId1"/>
     <sheet name="Sound" sheetId="2" r:id="rId2"/>
+    <sheet name="Questions" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
   <si>
     <t>main menu</t>
   </si>
@@ -239,6 +240,24 @@
   </si>
   <si>
     <t>มีมากกว่า 1 เพลงได้</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Nuttanon Prabaripay</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>น้ำ(ความชื้น) ของแปลงผัก อยู่ได้นานเท่าไร</t>
+  </si>
+  <si>
+    <t>ขอเปลี่ยนวิธีปลูกผักใหม่ ได้หรือไม่</t>
   </si>
 </sst>
 </file>
@@ -283,14 +302,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -309,6 +331,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -968,7 +997,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1001,7 +1030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93B43348-8BF1-4962-9048-F23A20CD6675}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1169,11 +1198,72 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="2" operator="beginsWith" text="0">
       <formula>LEFT(D1,LEN("0"))="0"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC3E692-DB7C-45C1-874C-1A95E759268E}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.75" customWidth="1"/>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="2" operator="beginsWith" text="0">
+      <formula>LEFT(D1,LEN("0"))="0"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>